<commit_message>
Solution to the #1 Problem
</commit_message>
<xml_diff>
--- a/problems.xlsx
+++ b/problems.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D33C48-057A-4782-BEB2-9799F3EDB187}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C862CE1-EB54-424F-BB58-94AB27E474CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{C50A9692-CF42-415B-8F57-AF5CC56BCA27}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Suppose we want to build a scheduling app. We have the times people are currently busy, e.g. 
 { 
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>File Name</t>
+  </si>
+  <si>
+    <t>MergeInterval.java</t>
   </si>
 </sst>
 </file>
@@ -78,7 +81,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,19 +89,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,24 +437,24 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
     <col min="2" max="2" width="91.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -441,8 +462,11 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>